<commit_message>
template cleanup, add country list
</commit_message>
<xml_diff>
--- a/fidesctl/src/fidesctl/templates/fides_datamap_template.xlsx
+++ b/fidesctl/src/fidesctl/templates/fides_datamap_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Art30 mock (WIP)" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Controller</t>
   </si>
@@ -23,12 +23,6 @@
   </si>
   <si>
     <t>Representative (if applicable)</t>
-  </si>
-  <si>
-    <t>Empty Column</t>
-  </si>
-  <si>
-    <t>Here</t>
   </si>
   <si>
     <t>Fides annotation</t>
@@ -167,7 +161,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border/>
     <border>
       <left style="thin">
@@ -206,17 +200,6 @@
       </bottom>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -241,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -268,27 +251,18 @@
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -300,14 +274,8 @@
     <xf borderId="3" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
@@ -666,12 +634,12 @@
     <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="12"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -697,15 +665,11 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="13" t="s">
-        <v>4</v>
-      </c>
+      <c r="I7" s="10"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="K7" s="10"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="13"/>
+      <c r="M7" s="10"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
@@ -718,117 +682,117 @@
       <c r="W7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16" t="s">
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="16" t="s">
+      <c r="V8" s="12"/>
+      <c r="W8" s="14"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="V8" s="15"/>
-      <c r="W8" s="17"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="18" t="s">
+      <c r="C9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="E9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="F9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="G9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="H9" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="I9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="J9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="K9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="L9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="M9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="20" t="s">
+      <c r="N9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="20" t="s">
+      <c r="O9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="P9" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="21" t="s">
+      <c r="Q9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="P9" s="21" t="s">
+      <c r="R9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="Q9" s="21" t="s">
+      <c r="S9" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="R9" s="21" t="s">
+      <c r="T9" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="S9" s="21" t="s">
+      <c r="U9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="T9" s="21" t="s">
+      <c r="V9" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="U9" s="21" t="s">
+      <c r="W9" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="V9" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="W9" s="21" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="10">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="23"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="8"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
@@ -847,8 +811,8 @@
       <c r="W10" s="9"/>
     </row>
     <row r="11">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -872,8 +836,8 @@
       <c r="W11" s="9"/>
     </row>
     <row r="12">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -897,8 +861,8 @@
       <c r="W12" s="9"/>
     </row>
     <row r="13">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -922,8 +886,8 @@
       <c r="W13" s="9"/>
     </row>
     <row r="14">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -947,8 +911,8 @@
       <c r="W14" s="9"/>
     </row>
     <row r="15">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -972,8 +936,8 @@
       <c r="W15" s="9"/>
     </row>
     <row r="16">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -997,8 +961,8 @@
       <c r="W16" s="9"/>
     </row>
     <row r="17">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -1022,8 +986,8 @@
       <c r="W17" s="9"/>
     </row>
     <row r="18">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -1047,8 +1011,8 @@
       <c r="W18" s="9"/>
     </row>
     <row r="19">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -1072,8 +1036,8 @@
       <c r="W19" s="9"/>
     </row>
     <row r="20">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -1097,8 +1061,8 @@
       <c r="W20" s="9"/>
     </row>
     <row r="21">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -1122,8 +1086,8 @@
       <c r="W21" s="9"/>
     </row>
     <row r="22">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -1147,8 +1111,8 @@
       <c r="W22" s="9"/>
     </row>
     <row r="23">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -1172,8 +1136,8 @@
       <c r="W23" s="9"/>
     </row>
     <row r="24">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -1197,8 +1161,8 @@
       <c r="W24" s="9"/>
     </row>
     <row r="25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -1222,8 +1186,8 @@
       <c r="W25" s="9"/>
     </row>
     <row r="26">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -1247,8 +1211,8 @@
       <c r="W26" s="9"/>
     </row>
     <row r="27">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -1272,8 +1236,8 @@
       <c r="W27" s="9"/>
     </row>
     <row r="28">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -1297,8 +1261,8 @@
       <c r="W28" s="9"/>
     </row>
     <row r="29">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -1322,8 +1286,8 @@
       <c r="W29" s="9"/>
     </row>
     <row r="30">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -1347,8 +1311,8 @@
       <c r="W30" s="9"/>
     </row>
     <row r="31">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -1372,8 +1336,8 @@
       <c r="W31" s="9"/>
     </row>
     <row r="32">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -1397,8 +1361,8 @@
       <c r="W32" s="9"/>
     </row>
     <row r="33">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -1422,8 +1386,8 @@
       <c r="W33" s="9"/>
     </row>
     <row r="34">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -1447,8 +1411,8 @@
       <c r="W34" s="9"/>
     </row>
     <row r="35">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -1472,8 +1436,8 @@
       <c r="W35" s="9"/>
     </row>
     <row r="36">
-      <c r="A36" s="24"/>
-      <c r="B36" s="24"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
@@ -1497,8 +1461,8 @@
       <c r="W36" s="9"/>
     </row>
     <row r="37">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -1522,8 +1486,8 @@
       <c r="W37" s="9"/>
     </row>
     <row r="38">
-      <c r="A38" s="24"/>
-      <c r="B38" s="24"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -1547,8 +1511,8 @@
       <c r="W38" s="9"/>
     </row>
     <row r="39">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
@@ -1572,8 +1536,8 @@
       <c r="W39" s="9"/>
     </row>
     <row r="40">
-      <c r="A40" s="24"/>
-      <c r="B40" s="24"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
@@ -1597,8 +1561,8 @@
       <c r="W40" s="9"/>
     </row>
     <row r="41">
-      <c r="A41" s="24"/>
-      <c r="B41" s="24"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
@@ -1622,8 +1586,8 @@
       <c r="W41" s="9"/>
     </row>
     <row r="42">
-      <c r="A42" s="24"/>
-      <c r="B42" s="24"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
@@ -1647,8 +1611,8 @@
       <c r="W42" s="9"/>
     </row>
     <row r="43">
-      <c r="A43" s="24"/>
-      <c r="B43" s="24"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -1672,8 +1636,8 @@
       <c r="W43" s="9"/>
     </row>
     <row r="44">
-      <c r="A44" s="24"/>
-      <c r="B44" s="24"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
@@ -1697,8 +1661,8 @@
       <c r="W44" s="9"/>
     </row>
     <row r="45">
-      <c r="A45" s="24"/>
-      <c r="B45" s="24"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
@@ -1722,8 +1686,8 @@
       <c r="W45" s="9"/>
     </row>
     <row r="46">
-      <c r="A46" s="24"/>
-      <c r="B46" s="24"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
@@ -1747,8 +1711,8 @@
       <c r="W46" s="9"/>
     </row>
     <row r="47">
-      <c r="A47" s="24"/>
-      <c r="B47" s="24"/>
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
@@ -1772,8 +1736,8 @@
       <c r="W47" s="9"/>
     </row>
     <row r="48">
-      <c r="A48" s="24"/>
-      <c r="B48" s="24"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
@@ -1797,8 +1761,8 @@
       <c r="W48" s="9"/>
     </row>
     <row r="49">
-      <c r="A49" s="24"/>
-      <c r="B49" s="24"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
@@ -1822,8 +1786,8 @@
       <c r="W49" s="9"/>
     </row>
     <row r="50">
-      <c r="A50" s="24"/>
-      <c r="B50" s="24"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
@@ -1847,8 +1811,8 @@
       <c r="W50" s="9"/>
     </row>
     <row r="51">
-      <c r="A51" s="24"/>
-      <c r="B51" s="24"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
@@ -1872,8 +1836,8 @@
       <c r="W51" s="9"/>
     </row>
     <row r="52">
-      <c r="A52" s="24"/>
-      <c r="B52" s="24"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
@@ -1897,8 +1861,8 @@
       <c r="W52" s="9"/>
     </row>
     <row r="53">
-      <c r="A53" s="24"/>
-      <c r="B53" s="24"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
@@ -1922,8 +1886,8 @@
       <c r="W53" s="9"/>
     </row>
     <row r="54">
-      <c r="A54" s="24"/>
-      <c r="B54" s="24"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
@@ -1947,8 +1911,8 @@
       <c r="W54" s="9"/>
     </row>
     <row r="55">
-      <c r="A55" s="24"/>
-      <c r="B55" s="24"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
@@ -1972,8 +1936,8 @@
       <c r="W55" s="9"/>
     </row>
     <row r="56">
-      <c r="A56" s="24"/>
-      <c r="B56" s="24"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
@@ -1997,8 +1961,8 @@
       <c r="W56" s="9"/>
     </row>
     <row r="57">
-      <c r="A57" s="24"/>
-      <c r="B57" s="24"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
@@ -2022,8 +1986,8 @@
       <c r="W57" s="9"/>
     </row>
     <row r="58">
-      <c r="A58" s="24"/>
-      <c r="B58" s="24"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
@@ -2047,8 +2011,8 @@
       <c r="W58" s="9"/>
     </row>
     <row r="59">
-      <c r="A59" s="24"/>
-      <c r="B59" s="24"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
@@ -2072,8 +2036,8 @@
       <c r="W59" s="9"/>
     </row>
     <row r="60">
-      <c r="A60" s="24"/>
-      <c r="B60" s="24"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
@@ -2097,8 +2061,8 @@
       <c r="W60" s="9"/>
     </row>
     <row r="61">
-      <c r="A61" s="24"/>
-      <c r="B61" s="24"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
@@ -2122,8 +2086,8 @@
       <c r="W61" s="9"/>
     </row>
     <row r="62">
-      <c r="A62" s="24"/>
-      <c r="B62" s="24"/>
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
@@ -2147,8 +2111,8 @@
       <c r="W62" s="9"/>
     </row>
     <row r="63">
-      <c r="A63" s="24"/>
-      <c r="B63" s="24"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
@@ -2172,8 +2136,8 @@
       <c r="W63" s="9"/>
     </row>
     <row r="64">
-      <c r="A64" s="24"/>
-      <c r="B64" s="24"/>
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
@@ -2197,8 +2161,8 @@
       <c r="W64" s="9"/>
     </row>
     <row r="65">
-      <c r="A65" s="24"/>
-      <c r="B65" s="24"/>
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
@@ -2222,8 +2186,8 @@
       <c r="W65" s="9"/>
     </row>
     <row r="66">
-      <c r="A66" s="24"/>
-      <c r="B66" s="24"/>
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
@@ -2247,8 +2211,8 @@
       <c r="W66" s="9"/>
     </row>
     <row r="67">
-      <c r="A67" s="24"/>
-      <c r="B67" s="24"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
       <c r="C67" s="9"/>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
@@ -2272,8 +2236,8 @@
       <c r="W67" s="9"/>
     </row>
     <row r="68">
-      <c r="A68" s="24"/>
-      <c r="B68" s="24"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
@@ -2297,8 +2261,8 @@
       <c r="W68" s="9"/>
     </row>
     <row r="69">
-      <c r="A69" s="24"/>
-      <c r="B69" s="24"/>
+      <c r="A69" s="9"/>
+      <c r="B69" s="9"/>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
@@ -2322,8 +2286,8 @@
       <c r="W69" s="9"/>
     </row>
     <row r="70">
-      <c r="A70" s="24"/>
-      <c r="B70" s="24"/>
+      <c r="A70" s="9"/>
+      <c r="B70" s="9"/>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
@@ -2347,8 +2311,8 @@
       <c r="W70" s="9"/>
     </row>
     <row r="71">
-      <c r="A71" s="24"/>
-      <c r="B71" s="24"/>
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
@@ -2372,8 +2336,8 @@
       <c r="W71" s="9"/>
     </row>
     <row r="72">
-      <c r="A72" s="24"/>
-      <c r="B72" s="24"/>
+      <c r="A72" s="9"/>
+      <c r="B72" s="9"/>
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
@@ -2397,8 +2361,8 @@
       <c r="W72" s="9"/>
     </row>
     <row r="73">
-      <c r="A73" s="24"/>
-      <c r="B73" s="24"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
@@ -2422,8 +2386,8 @@
       <c r="W73" s="9"/>
     </row>
     <row r="74">
-      <c r="A74" s="24"/>
-      <c r="B74" s="24"/>
+      <c r="A74" s="9"/>
+      <c r="B74" s="9"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
@@ -2447,8 +2411,8 @@
       <c r="W74" s="9"/>
     </row>
     <row r="75">
-      <c r="A75" s="24"/>
-      <c r="B75" s="24"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
@@ -2472,8 +2436,8 @@
       <c r="W75" s="9"/>
     </row>
     <row r="76">
-      <c r="A76" s="24"/>
-      <c r="B76" s="24"/>
+      <c r="A76" s="9"/>
+      <c r="B76" s="9"/>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
@@ -2497,8 +2461,8 @@
       <c r="W76" s="9"/>
     </row>
     <row r="77">
-      <c r="A77" s="24"/>
-      <c r="B77" s="24"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
       <c r="C77" s="9"/>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
@@ -2522,8 +2486,8 @@
       <c r="W77" s="9"/>
     </row>
     <row r="78">
-      <c r="A78" s="24"/>
-      <c r="B78" s="24"/>
+      <c r="A78" s="9"/>
+      <c r="B78" s="9"/>
       <c r="C78" s="9"/>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
@@ -2547,8 +2511,8 @@
       <c r="W78" s="9"/>
     </row>
     <row r="79">
-      <c r="A79" s="24"/>
-      <c r="B79" s="24"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
@@ -2572,8 +2536,8 @@
       <c r="W79" s="9"/>
     </row>
     <row r="80">
-      <c r="A80" s="24"/>
-      <c r="B80" s="24"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="9"/>
       <c r="C80" s="9"/>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
@@ -2597,8 +2561,8 @@
       <c r="W80" s="9"/>
     </row>
     <row r="81">
-      <c r="A81" s="24"/>
-      <c r="B81" s="24"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="9"/>
       <c r="C81" s="9"/>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
@@ -2622,8 +2586,8 @@
       <c r="W81" s="9"/>
     </row>
     <row r="82">
-      <c r="A82" s="24"/>
-      <c r="B82" s="24"/>
+      <c r="A82" s="9"/>
+      <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
@@ -2647,8 +2611,8 @@
       <c r="W82" s="9"/>
     </row>
     <row r="83">
-      <c r="A83" s="24"/>
-      <c r="B83" s="24"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="9"/>
       <c r="C83" s="9"/>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
@@ -2672,8 +2636,8 @@
       <c r="W83" s="9"/>
     </row>
     <row r="84">
-      <c r="A84" s="24"/>
-      <c r="B84" s="24"/>
+      <c r="A84" s="9"/>
+      <c r="B84" s="9"/>
       <c r="C84" s="9"/>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
@@ -2697,8 +2661,8 @@
       <c r="W84" s="9"/>
     </row>
     <row r="85">
-      <c r="A85" s="24"/>
-      <c r="B85" s="24"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="9"/>
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
@@ -2722,8 +2686,8 @@
       <c r="W85" s="9"/>
     </row>
     <row r="86">
-      <c r="A86" s="24"/>
-      <c r="B86" s="24"/>
+      <c r="A86" s="9"/>
+      <c r="B86" s="9"/>
       <c r="C86" s="9"/>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
@@ -2747,8 +2711,8 @@
       <c r="W86" s="9"/>
     </row>
     <row r="87">
-      <c r="A87" s="24"/>
-      <c r="B87" s="24"/>
+      <c r="A87" s="9"/>
+      <c r="B87" s="9"/>
       <c r="C87" s="9"/>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
@@ -2772,8 +2736,8 @@
       <c r="W87" s="9"/>
     </row>
     <row r="88">
-      <c r="A88" s="24"/>
-      <c r="B88" s="24"/>
+      <c r="A88" s="9"/>
+      <c r="B88" s="9"/>
       <c r="C88" s="9"/>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
@@ -2797,8 +2761,8 @@
       <c r="W88" s="9"/>
     </row>
     <row r="89">
-      <c r="A89" s="24"/>
-      <c r="B89" s="24"/>
+      <c r="A89" s="9"/>
+      <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
@@ -2822,8 +2786,8 @@
       <c r="W89" s="9"/>
     </row>
     <row r="90">
-      <c r="A90" s="24"/>
-      <c r="B90" s="24"/>
+      <c r="A90" s="9"/>
+      <c r="B90" s="9"/>
       <c r="C90" s="9"/>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
@@ -2847,8 +2811,8 @@
       <c r="W90" s="9"/>
     </row>
     <row r="91">
-      <c r="A91" s="24"/>
-      <c r="B91" s="24"/>
+      <c r="A91" s="9"/>
+      <c r="B91" s="9"/>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
@@ -2872,8 +2836,8 @@
       <c r="W91" s="9"/>
     </row>
     <row r="92">
-      <c r="A92" s="24"/>
-      <c r="B92" s="24"/>
+      <c r="A92" s="9"/>
+      <c r="B92" s="9"/>
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
@@ -2897,8 +2861,8 @@
       <c r="W92" s="9"/>
     </row>
     <row r="93">
-      <c r="A93" s="24"/>
-      <c r="B93" s="24"/>
+      <c r="A93" s="9"/>
+      <c r="B93" s="9"/>
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
@@ -2922,8 +2886,8 @@
       <c r="W93" s="9"/>
     </row>
     <row r="94">
-      <c r="A94" s="24"/>
-      <c r="B94" s="24"/>
+      <c r="A94" s="9"/>
+      <c r="B94" s="9"/>
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
@@ -2947,8 +2911,8 @@
       <c r="W94" s="9"/>
     </row>
     <row r="95">
-      <c r="A95" s="24"/>
-      <c r="B95" s="24"/>
+      <c r="A95" s="9"/>
+      <c r="B95" s="9"/>
       <c r="C95" s="9"/>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
@@ -2972,8 +2936,8 @@
       <c r="W95" s="9"/>
     </row>
     <row r="96">
-      <c r="A96" s="24"/>
-      <c r="B96" s="24"/>
+      <c r="A96" s="9"/>
+      <c r="B96" s="9"/>
       <c r="C96" s="9"/>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
@@ -2997,8 +2961,8 @@
       <c r="W96" s="9"/>
     </row>
     <row r="97">
-      <c r="A97" s="24"/>
-      <c r="B97" s="24"/>
+      <c r="A97" s="9"/>
+      <c r="B97" s="9"/>
       <c r="C97" s="9"/>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
@@ -3022,8 +2986,8 @@
       <c r="W97" s="9"/>
     </row>
     <row r="98">
-      <c r="A98" s="24"/>
-      <c r="B98" s="24"/>
+      <c r="A98" s="9"/>
+      <c r="B98" s="9"/>
       <c r="C98" s="9"/>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
@@ -3047,8 +3011,8 @@
       <c r="W98" s="9"/>
     </row>
     <row r="99">
-      <c r="A99" s="24"/>
-      <c r="B99" s="24"/>
+      <c r="A99" s="9"/>
+      <c r="B99" s="9"/>
       <c r="C99" s="9"/>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
@@ -3072,8 +3036,8 @@
       <c r="W99" s="9"/>
     </row>
     <row r="100">
-      <c r="A100" s="24"/>
-      <c r="B100" s="24"/>
+      <c r="A100" s="9"/>
+      <c r="B100" s="9"/>
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
@@ -3097,8 +3061,8 @@
       <c r="W100" s="9"/>
     </row>
     <row r="101">
-      <c r="A101" s="24"/>
-      <c r="B101" s="24"/>
+      <c r="A101" s="9"/>
+      <c r="B101" s="9"/>
       <c r="C101" s="9"/>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
@@ -3122,29 +3086,29 @@
       <c r="W101" s="9"/>
     </row>
     <row r="102">
-      <c r="A102" s="3"/>
-      <c r="B102" s="3"/>
-      <c r="C102" s="25"/>
-      <c r="D102" s="25"/>
-      <c r="E102" s="25"/>
-      <c r="F102" s="25"/>
-      <c r="G102" s="25"/>
-      <c r="H102" s="25"/>
-      <c r="I102" s="25"/>
-      <c r="J102" s="25"/>
-      <c r="K102" s="25"/>
-      <c r="L102" s="25"/>
-      <c r="M102" s="25"/>
-      <c r="N102" s="25"/>
-      <c r="O102" s="25"/>
-      <c r="P102" s="25"/>
-      <c r="Q102" s="25"/>
-      <c r="R102" s="25"/>
-      <c r="S102" s="25"/>
-      <c r="T102" s="25"/>
-      <c r="U102" s="25"/>
-      <c r="V102" s="25"/>
-      <c r="W102" s="25"/>
+      <c r="A102" s="20"/>
+      <c r="B102" s="20"/>
+      <c r="C102" s="20"/>
+      <c r="D102" s="20"/>
+      <c r="E102" s="20"/>
+      <c r="F102" s="20"/>
+      <c r="G102" s="20"/>
+      <c r="H102" s="20"/>
+      <c r="I102" s="20"/>
+      <c r="J102" s="20"/>
+      <c r="K102" s="20"/>
+      <c r="L102" s="20"/>
+      <c r="M102" s="20"/>
+      <c r="N102" s="20"/>
+      <c r="O102" s="20"/>
+      <c r="P102" s="20"/>
+      <c r="Q102" s="20"/>
+      <c r="R102" s="20"/>
+      <c r="S102" s="20"/>
+      <c r="T102" s="20"/>
+      <c r="U102" s="20"/>
+      <c r="V102" s="20"/>
+      <c r="W102" s="20"/>
     </row>
     <row r="103">
       <c r="A103" s="3"/>

</xml_diff>